<commit_message>
ls mp profile urls collected
</commit_message>
<xml_diff>
--- a/Resources/mp_track.xlsx
+++ b/Resources/mp_track.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -5954,8 +5954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" zoomScale="84" workbookViewId="0">
-      <selection activeCell="G428" sqref="G428"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,7 +5972,7 @@
     <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>

</xml_diff>